<commit_message>
fix: no notes for qiuck evaluation
</commit_message>
<xml_diff>
--- a/input/W4-IE-CLIvia-Generator.xlsx
+++ b/input/W4-IE-CLIvia-Generator.xlsx
@@ -1398,15 +1398,15 @@
       <name val="Arial"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -1678,10 +1678,13 @@
     <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1692,9 +1695,6 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -1729,13 +1729,13 @@
     <xf borderId="0" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment textRotation="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -1745,24 +1745,24 @@
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment textRotation="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="5" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="5" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="8" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="8" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment textRotation="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" textRotation="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="8" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="8" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1828,7 +1828,7 @@
     <xf borderId="0" fillId="10" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="10" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="10" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
@@ -1871,7 +1871,7 @@
     <xf borderId="0" fillId="11" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="11" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="11" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="11" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1889,7 +1889,7 @@
     <xf borderId="0" fillId="11" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="11" fontId="8" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="11" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -1923,7 +1923,7 @@
     <xf borderId="0" fillId="11" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2455,7 +2455,7 @@
       </c>
       <c r="D5" s="9">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E5" s="9">
         <f t="shared" si="1"/>
@@ -2913,7 +2913,7 @@
       </c>
       <c r="D7" s="10">
         <f t="shared" si="3"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E7" s="10">
         <f t="shared" si="3"/>
@@ -4917,7 +4917,7 @@
       </c>
       <c r="D18" s="27">
         <f t="shared" si="7"/>
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E18" s="27">
         <f t="shared" si="7"/>
@@ -5316,7 +5316,7 @@
         <v>3.0</v>
       </c>
       <c r="D20" s="29">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="E20" s="29">
         <v>0.0</v>
@@ -5835,7 +5835,7 @@
         <v>2.0</v>
       </c>
       <c r="D23" s="29">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E23" s="29">
         <v>2.0</v>
@@ -6527,7 +6527,7 @@
         <v>2.0</v>
       </c>
       <c r="D27" s="29">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="E27" s="29">
         <v>2.0</v>
@@ -6699,7 +6699,7 @@
       <c r="C28" s="29">
         <v>3.0</v>
       </c>
-      <c r="D28" s="29">
+      <c r="D28" s="30">
         <v>3.0</v>
       </c>
       <c r="E28" s="29">
@@ -7215,230 +7215,230 @@
       <c r="B31" s="10">
         <v>2.0</v>
       </c>
-      <c r="C31" s="30">
+      <c r="C31" s="31">
         <v>1.0</v>
       </c>
-      <c r="D31" s="30">
+      <c r="D31" s="31">
         <v>1.0</v>
       </c>
-      <c r="E31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="F31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="G31" s="30">
-        <v>0.0</v>
-      </c>
-      <c r="H31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="I31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="J31" s="30">
-        <v>0.0</v>
-      </c>
-      <c r="K31" s="30">
-        <v>0.0</v>
-      </c>
-      <c r="L31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="M31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="N31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="O31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="P31" s="30">
-        <v>0.0</v>
-      </c>
-      <c r="Q31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="R31" s="30">
-        <v>0.0</v>
-      </c>
-      <c r="S31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="T31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="U31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="V31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="W31" s="30">
-        <v>0.0</v>
-      </c>
-      <c r="X31" s="30">
-        <v>0.0</v>
-      </c>
-      <c r="Y31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="Z31" s="30">
-        <v>0.0</v>
-      </c>
-      <c r="AA31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="AB31" s="30">
-        <v>0.0</v>
-      </c>
-      <c r="AC31" s="30">
-        <v>0.0</v>
-      </c>
-      <c r="AD31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="AE31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="AF31" s="30">
-        <v>0.0</v>
-      </c>
-      <c r="AG31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="AH31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="AI31" s="30">
-        <v>0.0</v>
-      </c>
-      <c r="AJ31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="AK31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="AL31" s="30">
+      <c r="E31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="F31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="G31" s="31">
+        <v>0.0</v>
+      </c>
+      <c r="H31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="I31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="J31" s="31">
+        <v>0.0</v>
+      </c>
+      <c r="K31" s="31">
+        <v>0.0</v>
+      </c>
+      <c r="L31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="M31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="N31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="O31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="P31" s="31">
+        <v>0.0</v>
+      </c>
+      <c r="Q31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="R31" s="31">
+        <v>0.0</v>
+      </c>
+      <c r="S31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="T31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="U31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="V31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="W31" s="31">
+        <v>0.0</v>
+      </c>
+      <c r="X31" s="31">
+        <v>0.0</v>
+      </c>
+      <c r="Y31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="Z31" s="31">
+        <v>0.0</v>
+      </c>
+      <c r="AA31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="AB31" s="31">
+        <v>0.0</v>
+      </c>
+      <c r="AC31" s="31">
+        <v>0.0</v>
+      </c>
+      <c r="AD31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="AE31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="AF31" s="31">
+        <v>0.0</v>
+      </c>
+      <c r="AG31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="AH31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="AI31" s="31">
+        <v>0.0</v>
+      </c>
+      <c r="AJ31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="AK31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="AL31" s="31">
         <v>1.0</v>
       </c>
-      <c r="AM31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="AN31" s="30">
+      <c r="AM31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="AN31" s="31">
         <v>1.0</v>
       </c>
-      <c r="AO31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="AP31" s="30">
+      <c r="AO31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="AP31" s="31">
         <v>1.0</v>
       </c>
-      <c r="AQ31" s="30">
-        <v>0.0</v>
-      </c>
-      <c r="AR31" s="30">
-        <v>0.0</v>
-      </c>
-      <c r="AS31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="AT31" s="30">
+      <c r="AQ31" s="31">
+        <v>0.0</v>
+      </c>
+      <c r="AR31" s="31">
+        <v>0.0</v>
+      </c>
+      <c r="AS31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="AT31" s="31">
         <v>1.0</v>
       </c>
-      <c r="AU31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="AV31" s="30">
+      <c r="AU31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="AV31" s="31">
         <v>1.0</v>
       </c>
-      <c r="AW31" s="30">
-        <v>0.0</v>
-      </c>
-      <c r="AX31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="AY31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="AZ31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="BA31" s="30">
-        <v>0.0</v>
-      </c>
-      <c r="BB31" s="30">
-        <v>0.0</v>
-      </c>
-      <c r="BC31" s="30">
-        <v>2.0</v>
-      </c>
-      <c r="BD31" s="30">
-        <v>0.0</v>
-      </c>
-      <c r="BE31" s="30">
+      <c r="AW31" s="31">
+        <v>0.0</v>
+      </c>
+      <c r="AX31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="AY31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="AZ31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="BA31" s="31">
+        <v>0.0</v>
+      </c>
+      <c r="BB31" s="31">
+        <v>0.0</v>
+      </c>
+      <c r="BC31" s="31">
+        <v>2.0</v>
+      </c>
+      <c r="BD31" s="31">
+        <v>0.0</v>
+      </c>
+      <c r="BE31" s="31">
         <v>2.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="28"/>
       <c r="B32" s="10"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
-      <c r="L32" s="31"/>
-      <c r="M32" s="31"/>
-      <c r="N32" s="31"/>
-      <c r="O32" s="31"/>
-      <c r="P32" s="31"/>
-      <c r="Q32" s="31"/>
-      <c r="R32" s="31"/>
-      <c r="S32" s="31"/>
-      <c r="T32" s="31"/>
-      <c r="U32" s="31"/>
-      <c r="V32" s="31"/>
-      <c r="W32" s="31"/>
-      <c r="X32" s="31"/>
-      <c r="Y32" s="31"/>
-      <c r="Z32" s="31"/>
-      <c r="AA32" s="31"/>
-      <c r="AB32" s="31"/>
-      <c r="AC32" s="31"/>
-      <c r="AD32" s="31"/>
-      <c r="AE32" s="31"/>
-      <c r="AF32" s="31"/>
-      <c r="AG32" s="31"/>
-      <c r="AH32" s="31"/>
-      <c r="AI32" s="31"/>
-      <c r="AJ32" s="31"/>
-      <c r="AK32" s="31"/>
-      <c r="AL32" s="31"/>
-      <c r="AM32" s="31"/>
-      <c r="AN32" s="31"/>
-      <c r="AO32" s="31"/>
-      <c r="AP32" s="31"/>
-      <c r="AQ32" s="31"/>
-      <c r="AR32" s="31"/>
-      <c r="AS32" s="31"/>
-      <c r="AT32" s="31"/>
-      <c r="AU32" s="31"/>
-      <c r="AV32" s="31"/>
-      <c r="AW32" s="31"/>
-      <c r="AX32" s="31"/>
-      <c r="AY32" s="31"/>
-      <c r="AZ32" s="31"/>
-      <c r="BA32" s="31"/>
-      <c r="BB32" s="31"/>
-      <c r="BC32" s="31"/>
-      <c r="BD32" s="31"/>
-      <c r="BE32" s="31"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="32"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="32"/>
+      <c r="L32" s="32"/>
+      <c r="M32" s="32"/>
+      <c r="N32" s="32"/>
+      <c r="O32" s="32"/>
+      <c r="P32" s="32"/>
+      <c r="Q32" s="32"/>
+      <c r="R32" s="32"/>
+      <c r="S32" s="32"/>
+      <c r="T32" s="32"/>
+      <c r="U32" s="32"/>
+      <c r="V32" s="32"/>
+      <c r="W32" s="32"/>
+      <c r="X32" s="32"/>
+      <c r="Y32" s="32"/>
+      <c r="Z32" s="32"/>
+      <c r="AA32" s="32"/>
+      <c r="AB32" s="32"/>
+      <c r="AC32" s="32"/>
+      <c r="AD32" s="32"/>
+      <c r="AE32" s="32"/>
+      <c r="AF32" s="32"/>
+      <c r="AG32" s="32"/>
+      <c r="AH32" s="32"/>
+      <c r="AI32" s="32"/>
+      <c r="AJ32" s="32"/>
+      <c r="AK32" s="32"/>
+      <c r="AL32" s="32"/>
+      <c r="AM32" s="32"/>
+      <c r="AN32" s="32"/>
+      <c r="AO32" s="32"/>
+      <c r="AP32" s="32"/>
+      <c r="AQ32" s="32"/>
+      <c r="AR32" s="32"/>
+      <c r="AS32" s="32"/>
+      <c r="AT32" s="32"/>
+      <c r="AU32" s="32"/>
+      <c r="AV32" s="32"/>
+      <c r="AW32" s="32"/>
+      <c r="AX32" s="32"/>
+      <c r="AY32" s="32"/>
+      <c r="AZ32" s="32"/>
+      <c r="BA32" s="32"/>
+      <c r="BB32" s="32"/>
+      <c r="BC32" s="32"/>
+      <c r="BD32" s="32"/>
+      <c r="BE32" s="32"/>
     </row>
     <row r="33">
       <c r="A33" s="11" t="s">
@@ -8192,7 +8192,7 @@
       <c r="A37" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="B37" s="32">
+      <c r="B37" s="33">
         <v>2.0</v>
       </c>
       <c r="C37" s="29">
@@ -8364,29 +8364,29 @@
     <row r="38">
       <c r="A38" s="25"/>
       <c r="B38" s="10"/>
-      <c r="C38" s="33"/>
+      <c r="C38" s="34"/>
       <c r="D38" s="26"/>
-      <c r="E38" s="33"/>
+      <c r="E38" s="34"/>
       <c r="F38" s="26"/>
       <c r="G38" s="26"/>
-      <c r="H38" s="33"/>
+      <c r="H38" s="34"/>
       <c r="I38" s="26"/>
       <c r="J38" s="26"/>
       <c r="K38" s="26"/>
       <c r="L38" s="26"/>
       <c r="M38" s="26"/>
       <c r="N38" s="26"/>
-      <c r="O38" s="33"/>
+      <c r="O38" s="34"/>
       <c r="P38" s="26"/>
       <c r="Q38" s="26"/>
       <c r="R38" s="26"/>
-      <c r="S38" s="33"/>
-      <c r="T38" s="33"/>
+      <c r="S38" s="34"/>
+      <c r="T38" s="34"/>
       <c r="U38" s="26"/>
       <c r="V38" s="26"/>
       <c r="W38" s="26"/>
       <c r="X38" s="26"/>
-      <c r="Y38" s="33"/>
+      <c r="Y38" s="34"/>
       <c r="Z38" s="26"/>
       <c r="AA38" s="26"/>
       <c r="AB38" s="26"/>
@@ -8394,16 +8394,16 @@
       <c r="AD38" s="26"/>
       <c r="AE38" s="26"/>
       <c r="AF38" s="26"/>
-      <c r="AG38" s="33"/>
+      <c r="AG38" s="34"/>
       <c r="AH38" s="26"/>
       <c r="AI38" s="26"/>
-      <c r="AJ38" s="33"/>
+      <c r="AJ38" s="34"/>
       <c r="AK38" s="26"/>
-      <c r="AL38" s="33"/>
+      <c r="AL38" s="34"/>
       <c r="AM38" s="26"/>
       <c r="AN38" s="26"/>
       <c r="AO38" s="26"/>
-      <c r="AP38" s="33"/>
+      <c r="AP38" s="34"/>
       <c r="AQ38" s="26"/>
       <c r="AR38" s="26"/>
       <c r="AS38" s="26"/>
@@ -8421,8 +8421,8 @@
       <c r="BE38" s="26"/>
     </row>
     <row r="39">
-      <c r="A39" s="34"/>
-      <c r="B39" s="35" t="s">
+      <c r="A39" s="35"/>
+      <c r="B39" s="30" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="36">
@@ -8431,7 +8431,7 @@
       </c>
       <c r="D39" s="36">
         <f t="shared" si="9"/>
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="E39" s="36">
         <f t="shared" si="9"/>
@@ -8657,7 +8657,7 @@
       </c>
       <c r="D40" s="38">
         <f t="shared" si="10"/>
-        <v>0.8333333333</v>
+        <v>0.9666666667</v>
       </c>
       <c r="E40" s="39">
         <f t="shared" si="10"/>
@@ -8883,7 +8883,7 @@
       </c>
       <c r="D41" s="38">
         <f t="shared" si="11"/>
-        <v>0.8</v>
+        <v>0.88</v>
       </c>
       <c r="E41" s="38">
         <f t="shared" si="11"/>
@@ -9538,7 +9538,7 @@
       <c r="BE48" s="3"/>
     </row>
     <row r="49">
-      <c r="A49" s="35" t="s">
+      <c r="A49" s="30" t="s">
         <v>92</v>
       </c>
     </row>
@@ -9548,7 +9548,7 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="35" t="s">
+      <c r="A51" s="30" t="s">
         <v>94</v>
       </c>
     </row>
@@ -9595,10 +9595,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="48"/>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="30" t="s">
         <v>97</v>
       </c>
       <c r="F1" s="49" t="s">
@@ -9612,10 +9612,10 @@
       <c r="A2" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="35" t="b">
+      <c r="B2" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C2" s="35">
+      <c r="C2" s="30">
         <v>13.0</v>
       </c>
       <c r="J2" s="46"/>
@@ -9624,10 +9624,10 @@
       <c r="A3" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="35" t="b">
+      <c r="B3" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C3" s="35">
+      <c r="C3" s="30">
         <v>5.0</v>
       </c>
       <c r="F3" s="51" t="s">
@@ -9647,11 +9647,11 @@
       <c r="F4" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35" t="s">
+      <c r="H4" s="30"/>
+      <c r="I4" s="30" t="s">
         <v>101</v>
       </c>
     </row>
@@ -9659,23 +9659,23 @@
       <c r="A5" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="35" t="b">
+      <c r="B5" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C5" s="35">
+      <c r="C5" s="30">
         <v>1.0</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="30" t="s">
         <v>102</v>
       </c>
       <c r="F5" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35" t="s">
+      <c r="H5" s="30"/>
+      <c r="I5" s="30" t="s">
         <v>103</v>
       </c>
     </row>
@@ -9690,11 +9690,11 @@
       <c r="F6" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="H6" s="35"/>
-      <c r="I6" s="35" t="s">
+      <c r="H6" s="30"/>
+      <c r="I6" s="30" t="s">
         <v>104</v>
       </c>
     </row>
@@ -9702,20 +9702,20 @@
       <c r="A7" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="35" t="b">
+      <c r="B7" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C7" s="35">
+      <c r="C7" s="30">
         <v>15.0</v>
       </c>
       <c r="F7" s="54" t="s">
         <v>30</v>
       </c>
-      <c r="G7" s="35" t="s">
+      <c r="G7" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="H7" s="35"/>
-      <c r="I7" s="35" t="s">
+      <c r="H7" s="30"/>
+      <c r="I7" s="30" t="s">
         <v>105</v>
       </c>
     </row>
@@ -9723,19 +9723,19 @@
       <c r="A8" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="35" t="b">
+      <c r="B8" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C8" s="35">
+      <c r="C8" s="30">
         <v>3.0</v>
       </c>
       <c r="F8" s="56" t="s">
         <v>55</v>
       </c>
-      <c r="G8" s="35" t="s">
+      <c r="G8" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="30" t="s">
         <v>106</v>
       </c>
     </row>
@@ -9763,10 +9763,10 @@
       <c r="A11" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="35" t="b">
+      <c r="B11" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C11" s="35">
+      <c r="C11" s="30">
         <v>10.0</v>
       </c>
       <c r="F11" s="51" t="s">
@@ -9777,20 +9777,20 @@
       <c r="A12" s="48" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="35" t="b">
+      <c r="B12" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="30">
         <v>6.0</v>
       </c>
       <c r="F12" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="35" t="s">
+      <c r="G12" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="H12" s="35"/>
-      <c r="I12" s="35" t="s">
+      <c r="H12" s="30"/>
+      <c r="I12" s="30" t="s">
         <v>109</v>
       </c>
     </row>
@@ -9798,20 +9798,20 @@
       <c r="A13" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="35" t="b">
+      <c r="B13" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C13" s="35">
+      <c r="C13" s="30">
         <v>13.0</v>
       </c>
       <c r="F13" s="54" t="s">
         <v>59</v>
       </c>
-      <c r="G13" s="35" t="s">
+      <c r="G13" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35" t="s">
+      <c r="H13" s="30"/>
+      <c r="I13" s="30" t="s">
         <v>110</v>
       </c>
     </row>
@@ -9828,13 +9828,13 @@
       <c r="F14" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="35" t="s">
+      <c r="G14" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="H14" s="35" t="s">
+      <c r="H14" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="I14" s="35" t="s">
+      <c r="I14" s="30" t="s">
         <v>113</v>
       </c>
     </row>
@@ -9849,10 +9849,10 @@
       <c r="F15" s="57" t="s">
         <v>107</v>
       </c>
-      <c r="G15" s="35" t="s">
+      <c r="G15" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="H15" s="35"/>
+      <c r="H15" s="30"/>
       <c r="I15" s="59" t="s">
         <v>115</v>
       </c>
@@ -9861,19 +9861,19 @@
       <c r="A16" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="35" t="b">
+      <c r="B16" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C16" s="35">
+      <c r="C16" s="30">
         <v>16.0</v>
       </c>
       <c r="F16" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="G16" s="35" t="s">
+      <c r="G16" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="H16" s="35"/>
+      <c r="H16" s="30"/>
       <c r="I16" s="59" t="s">
         <v>116</v>
       </c>
@@ -9891,10 +9891,10 @@
       <c r="A18" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="35" t="b">
+      <c r="B18" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C18" s="35">
+      <c r="C18" s="30">
         <v>10.0</v>
       </c>
     </row>
@@ -9902,35 +9902,35 @@
       <c r="A19" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="35" t="b">
+      <c r="B19" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C19" s="35">
+      <c r="C19" s="30">
         <v>10.0</v>
       </c>
       <c r="F19" s="51" t="s">
         <v>117</v>
       </c>
-      <c r="G19" s="35"/>
-      <c r="H19" s="35"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
     </row>
     <row r="20">
       <c r="A20" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="35" t="b">
+      <c r="B20" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C20" s="35">
+      <c r="C20" s="30">
         <v>5.0</v>
       </c>
       <c r="F20" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="35" t="s">
+      <c r="G20" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="H20" s="35"/>
+      <c r="H20" s="30"/>
       <c r="I20" s="59" t="s">
         <v>119</v>
       </c>
@@ -9939,19 +9939,19 @@
       <c r="A21" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="35" t="b">
+      <c r="B21" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C21" s="35">
+      <c r="C21" s="30">
         <v>8.0</v>
       </c>
       <c r="F21" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="G21" s="35" t="s">
+      <c r="G21" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="H21" s="35"/>
+      <c r="H21" s="30"/>
       <c r="I21" s="59" t="s">
         <v>120</v>
       </c>
@@ -9972,11 +9972,11 @@
       <c r="F22" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="G22" s="35" t="s">
+      <c r="G22" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="H22" s="35"/>
-      <c r="I22" s="35" t="s">
+      <c r="H22" s="30"/>
+      <c r="I22" s="30" t="s">
         <v>122</v>
       </c>
     </row>
@@ -9991,11 +9991,11 @@
       <c r="F23" s="61" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="35" t="s">
+      <c r="G23" s="30" t="s">
         <v>118</v>
       </c>
-      <c r="H23" s="35"/>
-      <c r="I23" s="35" t="s">
+      <c r="H23" s="30"/>
+      <c r="I23" s="30" t="s">
         <v>123</v>
       </c>
     </row>
@@ -10003,19 +10003,19 @@
       <c r="A24" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="35" t="b">
+      <c r="B24" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C24" s="35">
+      <c r="C24" s="30">
         <v>7.0</v>
       </c>
       <c r="F24" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="G24" s="35" t="s">
+      <c r="G24" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="H24" s="35"/>
+      <c r="H24" s="30"/>
       <c r="I24" s="59" t="s">
         <v>124</v>
       </c>
@@ -10024,22 +10024,22 @@
       <c r="A25" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="35" t="b">
+      <c r="B25" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C25" s="35">
+      <c r="C25" s="30">
         <v>1.0</v>
       </c>
-      <c r="D25" s="35" t="s">
+      <c r="D25" s="30" t="s">
         <v>125</v>
       </c>
       <c r="F25" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="G25" s="35" t="s">
+      <c r="G25" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="H25" s="35"/>
+      <c r="H25" s="30"/>
       <c r="I25" s="59" t="s">
         <v>126</v>
       </c>
@@ -10070,10 +10070,10 @@
       <c r="A28" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="35" t="b">
+      <c r="B28" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C28" s="35">
+      <c r="C28" s="30">
         <v>6.0</v>
       </c>
       <c r="F28" s="51" t="s">
@@ -10084,20 +10084,20 @@
       <c r="A29" s="48" t="s">
         <v>36</v>
       </c>
-      <c r="B29" s="35" t="b">
+      <c r="B29" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C29" s="35">
+      <c r="C29" s="30">
         <v>5.0</v>
       </c>
       <c r="F29" s="52" t="s">
         <v>33</v>
       </c>
-      <c r="G29" s="35" t="s">
+      <c r="G29" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="H29" s="35"/>
-      <c r="I29" s="35" t="s">
+      <c r="H29" s="30"/>
+      <c r="I29" s="30" t="s">
         <v>128</v>
       </c>
     </row>
@@ -10105,10 +10105,10 @@
       <c r="A30" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="35" t="b">
+      <c r="B30" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C30" s="35">
+      <c r="C30" s="30">
         <v>9.0</v>
       </c>
     </row>
@@ -10127,13 +10127,13 @@
       <c r="A32" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="35" t="b">
+      <c r="B32" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C32" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="D32" s="35" t="s">
+      <c r="C32" s="30">
+        <v>2.0</v>
+      </c>
+      <c r="D32" s="30" t="s">
         <v>129</v>
       </c>
     </row>
@@ -10141,13 +10141,13 @@
       <c r="A33" s="48" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="35" t="b">
+      <c r="B33" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C33" s="35">
+      <c r="C33" s="30">
         <v>3.0</v>
       </c>
-      <c r="D33" s="35" t="s">
+      <c r="D33" s="30" t="s">
         <v>130</v>
       </c>
     </row>
@@ -10166,10 +10166,10 @@
       <c r="A35" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="35" t="b">
+      <c r="B35" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C35" s="35">
+      <c r="C35" s="30">
         <v>8.0</v>
       </c>
     </row>
@@ -10177,13 +10177,13 @@
       <c r="A36" s="48" t="s">
         <v>43</v>
       </c>
-      <c r="B36" s="35" t="b">
+      <c r="B36" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C36" s="35">
+      <c r="C36" s="30">
         <v>1.0</v>
       </c>
-      <c r="D36" s="35" t="s">
+      <c r="D36" s="30" t="s">
         <v>131</v>
       </c>
     </row>
@@ -10202,10 +10202,10 @@
       <c r="A38" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="35" t="b">
+      <c r="B38" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C38" s="35">
+      <c r="C38" s="30">
         <v>5.0</v>
       </c>
     </row>
@@ -10213,10 +10213,10 @@
       <c r="A39" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="35" t="b">
+      <c r="B39" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C39" s="35">
+      <c r="C39" s="30">
         <v>5.0</v>
       </c>
     </row>
@@ -10224,10 +10224,10 @@
       <c r="A40" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="B40" s="35" t="b">
+      <c r="B40" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C40" s="35">
+      <c r="C40" s="30">
         <v>4.0</v>
       </c>
     </row>
@@ -10235,10 +10235,10 @@
       <c r="A41" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="35" t="b">
+      <c r="B41" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C41" s="35">
+      <c r="C41" s="30">
         <v>4.0</v>
       </c>
     </row>
@@ -10246,10 +10246,10 @@
       <c r="A42" s="48" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="35" t="b">
+      <c r="B42" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C42" s="35">
+      <c r="C42" s="30">
         <v>6.0</v>
       </c>
     </row>
@@ -10271,10 +10271,10 @@
       <c r="A44" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="B44" s="35" t="b">
+      <c r="B44" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C44" s="35">
+      <c r="C44" s="30">
         <v>12.0</v>
       </c>
     </row>
@@ -10282,10 +10282,10 @@
       <c r="A45" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="B45" s="35" t="b">
+      <c r="B45" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C45" s="35">
+      <c r="C45" s="30">
         <v>35.0</v>
       </c>
     </row>
@@ -10293,13 +10293,13 @@
       <c r="A46" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="35" t="b">
+      <c r="B46" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C46" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="D46" s="35" t="s">
+      <c r="C46" s="30">
+        <v>2.0</v>
+      </c>
+      <c r="D46" s="30" t="s">
         <v>129</v>
       </c>
     </row>
@@ -10307,13 +10307,13 @@
       <c r="A47" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="B47" s="35" t="b">
+      <c r="B47" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C47" s="35">
+      <c r="C47" s="30">
         <v>3.0</v>
       </c>
-      <c r="D47" s="35" t="s">
+      <c r="D47" s="30" t="s">
         <v>133</v>
       </c>
     </row>
@@ -10330,13 +10330,13 @@
       <c r="A49" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="B49" s="35" t="b">
+      <c r="B49" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C49" s="35">
+      <c r="C49" s="30">
         <v>1.0</v>
       </c>
-      <c r="D49" s="35" t="s">
+      <c r="D49" s="30" t="s">
         <v>131</v>
       </c>
     </row>
@@ -10344,10 +10344,10 @@
       <c r="A50" s="48" t="s">
         <v>57</v>
       </c>
-      <c r="B50" s="35" t="b">
+      <c r="B50" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C50" s="35">
+      <c r="C50" s="30">
         <v>7.0</v>
       </c>
     </row>
@@ -10355,13 +10355,13 @@
       <c r="A51" s="48" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="35" t="b">
+      <c r="B51" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C51" s="35">
-        <v>2.0</v>
-      </c>
-      <c r="D51" s="35" t="s">
+      <c r="C51" s="30">
+        <v>2.0</v>
+      </c>
+      <c r="D51" s="30" t="s">
         <v>129</v>
       </c>
     </row>
@@ -10378,10 +10378,10 @@
       <c r="A53" s="48" t="s">
         <v>60</v>
       </c>
-      <c r="B53" s="35" t="b">
+      <c r="B53" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C53" s="35">
+      <c r="C53" s="30">
         <v>6.0</v>
       </c>
     </row>
@@ -10411,10 +10411,10 @@
       <c r="A56" s="48" t="s">
         <v>63</v>
       </c>
-      <c r="B56" s="35" t="b">
+      <c r="B56" s="30" t="b">
         <v>1</v>
       </c>
-      <c r="C56" s="35">
+      <c r="C56" s="30">
         <v>7.0</v>
       </c>
     </row>
@@ -10543,7 +10543,7 @@
       <c r="H4" s="71">
         <v>0.0</v>
       </c>
-      <c r="I4" s="33" t="b">
+      <c r="I4" s="34" t="b">
         <v>1</v>
       </c>
       <c r="J4" s="10">
@@ -10574,7 +10574,7 @@
       <c r="H5" s="71">
         <v>0.0</v>
       </c>
-      <c r="I5" s="33" t="b">
+      <c r="I5" s="34" t="b">
         <v>0</v>
       </c>
       <c r="J5" s="70">
@@ -10603,13 +10603,13 @@
       <c r="H6" s="71">
         <v>0.0</v>
       </c>
-      <c r="I6" s="33" t="b">
+      <c r="I6" s="34" t="b">
         <v>1</v>
       </c>
       <c r="J6" s="10">
         <v>0.0</v>
       </c>
-      <c r="K6" s="35" t="s">
+      <c r="K6" s="30" t="s">
         <v>154</v>
       </c>
     </row>
@@ -10630,13 +10630,13 @@
       <c r="H7" s="71">
         <v>0.0</v>
       </c>
-      <c r="I7" s="33" t="b">
+      <c r="I7" s="34" t="b">
         <v>1</v>
       </c>
       <c r="J7" s="10">
         <v>0.0</v>
       </c>
-      <c r="K7" s="35" t="s">
+      <c r="K7" s="30" t="s">
         <v>109</v>
       </c>
     </row>
@@ -10659,7 +10659,7 @@
       <c r="H8" s="71">
         <v>0.67</v>
       </c>
-      <c r="I8" s="33" t="b">
+      <c r="I8" s="34" t="b">
         <v>1</v>
       </c>
       <c r="J8" s="10">
@@ -10812,7 +10812,7 @@
       <c r="H13" s="71">
         <v>0.0</v>
       </c>
-      <c r="I13" s="33" t="b">
+      <c r="I13" s="34" t="b">
         <v>1</v>
       </c>
       <c r="J13" s="10">
@@ -10832,7 +10832,7 @@
       <c r="C14" s="69" t="s">
         <v>158</v>
       </c>
-      <c r="D14" s="35" t="s">
+      <c r="D14" s="30" t="s">
         <v>166</v>
       </c>
       <c r="E14" s="72"/>
@@ -11202,10 +11202,10 @@
       <c r="H25" s="71">
         <v>0.8</v>
       </c>
-      <c r="I25" s="33" t="b">
-        <v>0</v>
-      </c>
-      <c r="J25" s="32">
+      <c r="I25" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="J25" s="33">
         <v>2.0</v>
       </c>
       <c r="K25" s="7" t="s">
@@ -11238,7 +11238,7 @@
       <c r="I26" s="84" t="b">
         <v>0</v>
       </c>
-      <c r="J26" s="32">
+      <c r="J26" s="33">
         <v>2.0</v>
       </c>
       <c r="K26" s="7" t="s">
@@ -11271,7 +11271,7 @@
       <c r="I27" s="84" t="b">
         <v>0</v>
       </c>
-      <c r="J27" s="32">
+      <c r="J27" s="33">
         <v>1.0</v>
       </c>
       <c r="K27" s="7" t="s">
@@ -11366,7 +11366,7 @@
       <c r="I30" s="84" t="b">
         <v>0</v>
       </c>
-      <c r="J30" s="32">
+      <c r="J30" s="33">
         <v>1.0</v>
       </c>
       <c r="K30" s="7" t="s">
@@ -11454,7 +11454,7 @@
       <c r="H33" s="71">
         <v>0.73</v>
       </c>
-      <c r="I33" s="33" t="b">
+      <c r="I33" s="34" t="b">
         <v>1</v>
       </c>
       <c r="J33" s="10">
@@ -11561,13 +11561,13 @@
     </row>
     <row r="37">
       <c r="A37" s="23" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B37" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="C37" s="87" t="s">
-        <v>158</v>
+      <c r="C37" s="69" t="s">
+        <v>164</v>
       </c>
       <c r="D37" s="25" t="s">
         <v>218</v>
@@ -11704,7 +11704,7 @@
       <c r="H41" s="71">
         <v>0.87</v>
       </c>
-      <c r="I41" s="33" t="b">
+      <c r="I41" s="34" t="b">
         <v>1</v>
       </c>
       <c r="J41" s="70">
@@ -11890,10 +11890,10 @@
       <c r="H47" s="71">
         <v>0.77</v>
       </c>
-      <c r="I47" s="33" t="b">
+      <c r="I47" s="34" t="b">
         <v>1</v>
       </c>
-      <c r="J47" s="32">
+      <c r="J47" s="33">
         <v>1.0</v>
       </c>
       <c r="K47" s="3"/>
@@ -11946,7 +11946,7 @@
       <c r="H49" s="71">
         <v>0.87</v>
       </c>
-      <c r="I49" s="33" t="b">
+      <c r="I49" s="34" t="b">
         <v>1</v>
       </c>
       <c r="J49" s="10">
@@ -12019,8 +12019,8 @@
       <c r="K51" s="72"/>
     </row>
     <row r="52">
-      <c r="A52" s="25" t="b">
-        <v>0</v>
+      <c r="A52" s="23" t="b">
+        <v>1</v>
       </c>
       <c r="B52" s="25" t="s">
         <v>239</v>
@@ -12191,7 +12191,7 @@
       <c r="I57" s="84" t="b">
         <v>0</v>
       </c>
-      <c r="J57" s="32">
+      <c r="J57" s="33">
         <v>2.0</v>
       </c>
       <c r="K57" s="7" t="s">

</xml_diff>